<commit_message>
Last version with OCR improvement
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Référence</t>
   </si>
@@ -32,102 +32,69 @@
     <t>DRAM</t>
   </si>
   <si>
-    <t>H057</t>
-  </si>
-  <si>
-    <t>H094</t>
-  </si>
-  <si>
-    <t>H112</t>
-  </si>
-  <si>
-    <t>H132</t>
-  </si>
-  <si>
-    <t>J193</t>
-  </si>
-  <si>
-    <t>H100</t>
-  </si>
-  <si>
-    <t>H190</t>
-  </si>
-  <si>
-    <t>H590#90G0</t>
-  </si>
-  <si>
-    <t>J541#60VN</t>
-  </si>
-  <si>
-    <t>J560#BX71</t>
-  </si>
-  <si>
-    <t>J561#658K</t>
-  </si>
-  <si>
-    <t>J571#658M</t>
-  </si>
-  <si>
-    <t>J575#659A</t>
-  </si>
-  <si>
-    <t>H501#G401</t>
-  </si>
-  <si>
-    <t>H510#B11</t>
-  </si>
-  <si>
-    <t>H990#32K</t>
-  </si>
-  <si>
-    <t>J664</t>
-  </si>
-  <si>
-    <t>J685</t>
-  </si>
-  <si>
-    <t>J704</t>
-  </si>
-  <si>
-    <t>J738#8M</t>
-  </si>
-  <si>
-    <t>J739#512K</t>
+    <t>H501#G103</t>
+  </si>
+  <si>
+    <t>J580</t>
+  </si>
+  <si>
+    <t>J749</t>
+  </si>
+  <si>
+    <t>S728</t>
+  </si>
+  <si>
+    <t>S985</t>
   </si>
   <si>
     <t>J801</t>
   </si>
   <si>
-    <t>J802#4</t>
+    <t>J802#11</t>
   </si>
   <si>
     <t>J803</t>
   </si>
   <si>
+    <t>J804</t>
+  </si>
+  <si>
     <t>J807</t>
   </si>
   <si>
     <t>J819</t>
   </si>
   <si>
-    <t>J824</t>
-  </si>
-  <si>
     <t>J828</t>
   </si>
   <si>
     <t>J829</t>
   </si>
   <si>
+    <t>J830</t>
+  </si>
+  <si>
     <t>J835</t>
   </si>
   <si>
+    <t>J836</t>
+  </si>
+  <si>
     <t>J838</t>
   </si>
   <si>
     <t>J841</t>
   </si>
   <si>
+    <t>J842</t>
+  </si>
+  <si>
+    <t>J846</t>
+  </si>
+  <si>
+    <t>J848</t>
+  </si>
+  <si>
     <t>J850</t>
   </si>
   <si>
@@ -143,15 +110,18 @@
     <t>J876</t>
   </si>
   <si>
+    <t>J882</t>
+  </si>
+  <si>
     <t>J887</t>
   </si>
   <si>
-    <t>J888</t>
-  </si>
-  <si>
     <t>J890</t>
   </si>
   <si>
+    <t>J893</t>
+  </si>
+  <si>
     <t>J894</t>
   </si>
   <si>
@@ -164,58 +134,34 @@
     <t>J913</t>
   </si>
   <si>
-    <t>J927</t>
+    <t>J917</t>
   </si>
   <si>
     <t>J930</t>
   </si>
   <si>
-    <t>J935</t>
-  </si>
-  <si>
     <t>J937</t>
   </si>
   <si>
-    <t>J945</t>
-  </si>
-  <si>
-    <t>J953</t>
+    <t>J948</t>
+  </si>
+  <si>
+    <t>v953</t>
   </si>
   <si>
     <t>J956</t>
   </si>
   <si>
+    <t>J965</t>
+  </si>
+  <si>
     <t>J971</t>
   </si>
   <si>
-    <t>J972</t>
-  </si>
-  <si>
-    <t>R521</t>
-  </si>
-  <si>
-    <t>S615</t>
-  </si>
-  <si>
-    <t>S637</t>
-  </si>
-  <si>
-    <t>S707</t>
-  </si>
-  <si>
-    <t>S801#1</t>
-  </si>
-  <si>
-    <t>S808</t>
-  </si>
-  <si>
-    <t>S836#1</t>
-  </si>
-  <si>
-    <t>S837#1</t>
-  </si>
-  <si>
-    <t>S838#M</t>
+    <t>J981</t>
+  </si>
+  <si>
+    <t>R955</t>
   </si>
 </sst>
 </file>
@@ -547,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -566,36 +512,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -603,7 +519,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -625,277 +541,217 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last version with big improvement : 1. Three pytesseract 2. Comparaison of those three results 3. Genetical decision (group always win)
TO DO : finish the decision part
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Référence</t>
   </si>
@@ -32,136 +32,58 @@
     <t>DRAM</t>
   </si>
   <si>
-    <t>H501#G103</t>
-  </si>
-  <si>
-    <t>J580</t>
-  </si>
-  <si>
-    <t>J749</t>
-  </si>
-  <si>
-    <t>S728</t>
-  </si>
-  <si>
-    <t>S985</t>
-  </si>
-  <si>
-    <t>J801</t>
-  </si>
-  <si>
-    <t>J802#11</t>
-  </si>
-  <si>
-    <t>J803</t>
-  </si>
-  <si>
-    <t>J804</t>
-  </si>
-  <si>
-    <t>J807</t>
-  </si>
-  <si>
-    <t>J819</t>
-  </si>
-  <si>
-    <t>J828</t>
-  </si>
-  <si>
-    <t>J829</t>
-  </si>
-  <si>
-    <t>J830</t>
-  </si>
-  <si>
-    <t>J835</t>
-  </si>
-  <si>
-    <t>J836</t>
-  </si>
-  <si>
-    <t>J838</t>
-  </si>
-  <si>
-    <t>J841</t>
-  </si>
-  <si>
-    <t>J842</t>
-  </si>
-  <si>
-    <t>J846</t>
-  </si>
-  <si>
-    <t>J848</t>
-  </si>
-  <si>
-    <t>J850</t>
-  </si>
-  <si>
-    <t>J853</t>
-  </si>
-  <si>
-    <t>J854</t>
-  </si>
-  <si>
-    <t>J873</t>
-  </si>
-  <si>
-    <t>J876</t>
-  </si>
-  <si>
-    <t>J882</t>
-  </si>
-  <si>
-    <t>J887</t>
-  </si>
-  <si>
-    <t>J890</t>
-  </si>
-  <si>
-    <t>J893</t>
-  </si>
-  <si>
-    <t>J894</t>
-  </si>
-  <si>
-    <t>J895</t>
-  </si>
-  <si>
-    <t>J900</t>
-  </si>
-  <si>
-    <t>J913</t>
-  </si>
-  <si>
-    <t>J917</t>
-  </si>
-  <si>
-    <t>J930</t>
-  </si>
-  <si>
-    <t>J937</t>
-  </si>
-  <si>
-    <t>J948</t>
-  </si>
-  <si>
-    <t>v953</t>
-  </si>
-  <si>
-    <t>J956</t>
-  </si>
-  <si>
-    <t>J965</t>
-  </si>
-  <si>
-    <t>J971</t>
-  </si>
-  <si>
-    <t>J981</t>
-  </si>
-  <si>
-    <t>R955</t>
+    <t>H580#40</t>
+  </si>
+  <si>
+    <t>H590#90</t>
+  </si>
+  <si>
+    <t>J535#65</t>
+  </si>
+  <si>
+    <t>J562#65</t>
+  </si>
+  <si>
+    <t>J541#60</t>
+  </si>
+  <si>
+    <t>J571#65</t>
+  </si>
+  <si>
+    <t>J572#65</t>
+  </si>
+  <si>
+    <t>J599#65</t>
+  </si>
+  <si>
+    <t>H501#G1</t>
+  </si>
+  <si>
+    <t>H510#B</t>
+  </si>
+  <si>
+    <t>H990#3</t>
+  </si>
+  <si>
+    <t>J738#</t>
+  </si>
+  <si>
+    <t>J802#</t>
+  </si>
+  <si>
+    <t>S801</t>
+  </si>
+  <si>
+    <t>S837</t>
+  </si>
+  <si>
+    <t>S836</t>
+  </si>
+  <si>
+    <t>S838</t>
+  </si>
+  <si>
+    <t>S874#1</t>
   </si>
 </sst>
 </file>
@@ -493,7 +415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,11 +429,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -519,7 +436,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -541,217 +458,92 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V2.0.0 : --> ROI selection --> Tkinter Interface when text is not correctly detected --> Improvement of the results of Tesseract because of manipulation of the dpi & resolution
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Référence</t>
   </si>
@@ -50,40 +50,19 @@
     <t>J571#65</t>
   </si>
   <si>
-    <t>J572#65</t>
-  </si>
-  <si>
     <t>J599#65</t>
   </si>
   <si>
-    <t>H501#G1</t>
-  </si>
-  <si>
-    <t>H510#B</t>
-  </si>
-  <si>
     <t>H990#3</t>
   </si>
   <si>
     <t>J738#</t>
   </si>
   <si>
-    <t>J802#</t>
-  </si>
-  <si>
-    <t>S801</t>
-  </si>
-  <si>
-    <t>S837</t>
-  </si>
-  <si>
     <t>S836</t>
   </si>
   <si>
     <t>S838</t>
-  </si>
-  <si>
-    <t>S874#1</t>
   </si>
 </sst>
 </file>
@@ -436,7 +415,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -511,41 +490,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
V2.1.0 : --> Tkinter for confirmation of the user when mismatching of ref is okay --> TODO : compute score (0-100%) between regex and the three strings --> TODO : if 2 strings agree at 100% skip the tkinter part
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
   <si>
     <t>Référence</t>
   </si>
@@ -32,37 +32,274 @@
     <t>DRAM</t>
   </si>
   <si>
-    <t>H580#40</t>
-  </si>
-  <si>
-    <t>H590#90</t>
-  </si>
-  <si>
-    <t>J535#65</t>
-  </si>
-  <si>
-    <t>J562#65</t>
-  </si>
-  <si>
-    <t>J541#60</t>
-  </si>
-  <si>
-    <t>J571#65</t>
-  </si>
-  <si>
-    <t>J599#65</t>
-  </si>
-  <si>
-    <t>H990#3</t>
-  </si>
-  <si>
-    <t>J738#</t>
-  </si>
-  <si>
-    <t>S836</t>
-  </si>
-  <si>
-    <t>S838</t>
+    <t>H010</t>
+  </si>
+  <si>
+    <t>H048</t>
+  </si>
+  <si>
+    <t>H060</t>
+  </si>
+  <si>
+    <t>H089</t>
+  </si>
+  <si>
+    <t>H115</t>
+  </si>
+  <si>
+    <t>J146</t>
+  </si>
+  <si>
+    <t>J193</t>
+  </si>
+  <si>
+    <t>J311</t>
+  </si>
+  <si>
+    <t>H190</t>
+  </si>
+  <si>
+    <t>H200</t>
+  </si>
+  <si>
+    <t>H024</t>
+  </si>
+  <si>
+    <t>H201</t>
+  </si>
+  <si>
+    <t>H211</t>
+  </si>
+  <si>
+    <t>H302</t>
+  </si>
+  <si>
+    <t>H351</t>
+  </si>
+  <si>
+    <t>H402</t>
+  </si>
+  <si>
+    <t>J001</t>
+  </si>
+  <si>
+    <t>J013</t>
+  </si>
+  <si>
+    <t>J580</t>
+  </si>
+  <si>
+    <t>J858</t>
+  </si>
+  <si>
+    <t>J900</t>
+  </si>
+  <si>
+    <t>H580#40A0</t>
+  </si>
+  <si>
+    <t>H590#90E0</t>
+  </si>
+  <si>
+    <t>J535#655B</t>
+  </si>
+  <si>
+    <t>J541#60V8</t>
+  </si>
+  <si>
+    <t>J562#6552</t>
+  </si>
+  <si>
+    <t>J571#656E</t>
+  </si>
+  <si>
+    <t>J572#656F</t>
+  </si>
+  <si>
+    <t>J599#6569</t>
+  </si>
+  <si>
+    <t>H501#G103</t>
+  </si>
+  <si>
+    <t>H510#B11</t>
+  </si>
+  <si>
+    <t>H990#32K</t>
+  </si>
+  <si>
+    <t>J674</t>
+  </si>
+  <si>
+    <t>J721</t>
+  </si>
+  <si>
+    <t>J728</t>
+  </si>
+  <si>
+    <t>J733</t>
+  </si>
+  <si>
+    <t>J734</t>
+  </si>
+  <si>
+    <t>J736</t>
+  </si>
+  <si>
+    <t>J738#2M</t>
+  </si>
+  <si>
+    <t>J749</t>
+  </si>
+  <si>
+    <t>J801</t>
+  </si>
+  <si>
+    <t>J802#11</t>
+  </si>
+  <si>
+    <t>J803</t>
+  </si>
+  <si>
+    <t>J804</t>
+  </si>
+  <si>
+    <t>J807</t>
+  </si>
+  <si>
+    <t>J819</t>
+  </si>
+  <si>
+    <t>J828</t>
+  </si>
+  <si>
+    <t>J829</t>
+  </si>
+  <si>
+    <t>J835</t>
+  </si>
+  <si>
+    <t>J830</t>
+  </si>
+  <si>
+    <t>J836</t>
+  </si>
+  <si>
+    <t>J838</t>
+  </si>
+  <si>
+    <t>J841</t>
+  </si>
+  <si>
+    <t>J842</t>
+  </si>
+  <si>
+    <t>J850</t>
+  </si>
+  <si>
+    <t>J853</t>
+  </si>
+  <si>
+    <t>J854</t>
+  </si>
+  <si>
+    <t>J873</t>
+  </si>
+  <si>
+    <t>J876</t>
+  </si>
+  <si>
+    <t>J882</t>
+  </si>
+  <si>
+    <t>J887</t>
+  </si>
+  <si>
+    <t>J890</t>
+  </si>
+  <si>
+    <t>J894</t>
+  </si>
+  <si>
+    <t>J895</t>
+  </si>
+  <si>
+    <t>J913</t>
+  </si>
+  <si>
+    <t>J917</t>
+  </si>
+  <si>
+    <t>J930</t>
+  </si>
+  <si>
+    <t>J937</t>
+  </si>
+  <si>
+    <t>J953</t>
+  </si>
+  <si>
+    <t>J956</t>
+  </si>
+  <si>
+    <t>J965</t>
+  </si>
+  <si>
+    <t>J971</t>
+  </si>
+  <si>
+    <t>J981</t>
+  </si>
+  <si>
+    <t>R955</t>
+  </si>
+  <si>
+    <t>S617</t>
+  </si>
+  <si>
+    <t>S643</t>
+  </si>
+  <si>
+    <t>S656</t>
+  </si>
+  <si>
+    <t>S661</t>
+  </si>
+  <si>
+    <t>S728</t>
+  </si>
+  <si>
+    <t>S707</t>
+  </si>
+  <si>
+    <t>S731</t>
+  </si>
+  <si>
+    <t>S737</t>
+  </si>
+  <si>
+    <t>S801#2</t>
+  </si>
+  <si>
+    <t>S807</t>
+  </si>
+  <si>
+    <t>S836#1</t>
+  </si>
+  <si>
+    <t>S837#1</t>
+  </si>
+  <si>
+    <t>S838#M</t>
+  </si>
+  <si>
+    <t>S841</t>
+  </si>
+  <si>
+    <t>S874#16K</t>
+  </si>
+  <si>
+    <t>S985</t>
   </si>
 </sst>
 </file>
@@ -394,7 +631,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,6 +645,101 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -415,7 +747,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -437,57 +769,362 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V2.2.0 : --> TODO : improve the detection of text with pytesseract
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Référence</t>
   </si>
@@ -32,274 +32,190 @@
     <t>DRAM</t>
   </si>
   <si>
-    <t>H010</t>
-  </si>
-  <si>
-    <t>H048</t>
-  </si>
-  <si>
-    <t>H060</t>
-  </si>
-  <si>
-    <t>H089</t>
-  </si>
-  <si>
-    <t>H115</t>
-  </si>
-  <si>
-    <t>J146</t>
+    <t>H013</t>
+  </si>
+  <si>
+    <t>H057</t>
+  </si>
+  <si>
+    <t>H094</t>
+  </si>
+  <si>
+    <t>H112</t>
+  </si>
+  <si>
+    <t>H132</t>
   </si>
   <si>
     <t>J193</t>
   </si>
   <si>
-    <t>J311</t>
+    <t>H100</t>
   </si>
   <si>
     <t>H190</t>
   </si>
   <si>
-    <t>H200</t>
-  </si>
-  <si>
-    <t>H024</t>
-  </si>
-  <si>
-    <t>H201</t>
-  </si>
-  <si>
-    <t>H211</t>
-  </si>
-  <si>
-    <t>H302</t>
-  </si>
-  <si>
-    <t>H351</t>
-  </si>
-  <si>
-    <t>H402</t>
-  </si>
-  <si>
-    <t>J001</t>
-  </si>
-  <si>
-    <t>J013</t>
-  </si>
-  <si>
-    <t>J580</t>
-  </si>
-  <si>
-    <t>J858</t>
+    <t>H580#40A5</t>
+  </si>
+  <si>
+    <t>H590#90G0</t>
+  </si>
+  <si>
+    <t>J541#60VN</t>
+  </si>
+  <si>
+    <t>J560#BX7</t>
+  </si>
+  <si>
+    <t>J561#658K</t>
+  </si>
+  <si>
+    <t>J571#658M</t>
+  </si>
+  <si>
+    <t>H501#G401</t>
+  </si>
+  <si>
+    <t>J575#659A</t>
+  </si>
+  <si>
+    <t>H510#B11</t>
+  </si>
+  <si>
+    <t>H990#32K</t>
+  </si>
+  <si>
+    <t>J664</t>
+  </si>
+  <si>
+    <t>J685</t>
+  </si>
+  <si>
+    <t>J704</t>
+  </si>
+  <si>
+    <t>J738#8M</t>
+  </si>
+  <si>
+    <t>J739#5</t>
+  </si>
+  <si>
+    <t>J801</t>
+  </si>
+  <si>
+    <t>J802#4</t>
+  </si>
+  <si>
+    <t>J803</t>
+  </si>
+  <si>
+    <t>J807</t>
+  </si>
+  <si>
+    <t>J819</t>
+  </si>
+  <si>
+    <t>J824</t>
+  </si>
+  <si>
+    <t>J829</t>
+  </si>
+  <si>
+    <t>J828</t>
+  </si>
+  <si>
+    <t>J835</t>
+  </si>
+  <si>
+    <t>J838</t>
+  </si>
+  <si>
+    <t>J841</t>
+  </si>
+  <si>
+    <t>J850</t>
+  </si>
+  <si>
+    <t>J853</t>
+  </si>
+  <si>
+    <t>J854</t>
+  </si>
+  <si>
+    <t>J873</t>
+  </si>
+  <si>
+    <t>J876</t>
+  </si>
+  <si>
+    <t>J887</t>
+  </si>
+  <si>
+    <t>J888</t>
+  </si>
+  <si>
+    <t>J890</t>
+  </si>
+  <si>
+    <t>J893</t>
+  </si>
+  <si>
+    <t>J894</t>
+  </si>
+  <si>
+    <t>J895</t>
   </si>
   <si>
     <t>J900</t>
   </si>
   <si>
-    <t>H580#40A0</t>
-  </si>
-  <si>
-    <t>H590#90E0</t>
-  </si>
-  <si>
-    <t>J535#655B</t>
-  </si>
-  <si>
-    <t>J541#60V8</t>
-  </si>
-  <si>
-    <t>J562#6552</t>
-  </si>
-  <si>
-    <t>J571#656E</t>
-  </si>
-  <si>
-    <t>J572#656F</t>
-  </si>
-  <si>
-    <t>J599#6569</t>
-  </si>
-  <si>
-    <t>H501#G103</t>
-  </si>
-  <si>
-    <t>H510#B11</t>
-  </si>
-  <si>
-    <t>H990#32K</t>
-  </si>
-  <si>
-    <t>J674</t>
-  </si>
-  <si>
-    <t>J721</t>
-  </si>
-  <si>
-    <t>J728</t>
-  </si>
-  <si>
-    <t>J733</t>
-  </si>
-  <si>
-    <t>J734</t>
-  </si>
-  <si>
-    <t>J736</t>
-  </si>
-  <si>
-    <t>J738#2M</t>
-  </si>
-  <si>
-    <t>J749</t>
-  </si>
-  <si>
-    <t>J801</t>
-  </si>
-  <si>
-    <t>J802#11</t>
-  </si>
-  <si>
-    <t>J803</t>
-  </si>
-  <si>
-    <t>J804</t>
-  </si>
-  <si>
-    <t>J807</t>
-  </si>
-  <si>
-    <t>J819</t>
-  </si>
-  <si>
-    <t>J828</t>
-  </si>
-  <si>
-    <t>J829</t>
-  </si>
-  <si>
-    <t>J835</t>
-  </si>
-  <si>
-    <t>J830</t>
-  </si>
-  <si>
-    <t>J836</t>
-  </si>
-  <si>
-    <t>J838</t>
-  </si>
-  <si>
-    <t>J841</t>
-  </si>
-  <si>
-    <t>J842</t>
-  </si>
-  <si>
-    <t>J850</t>
-  </si>
-  <si>
-    <t>J853</t>
-  </si>
-  <si>
-    <t>J854</t>
-  </si>
-  <si>
-    <t>J873</t>
-  </si>
-  <si>
-    <t>J876</t>
-  </si>
-  <si>
-    <t>J882</t>
-  </si>
-  <si>
-    <t>J887</t>
-  </si>
-  <si>
-    <t>J890</t>
-  </si>
-  <si>
-    <t>J894</t>
-  </si>
-  <si>
-    <t>J895</t>
-  </si>
-  <si>
     <t>J913</t>
   </si>
   <si>
-    <t>J917</t>
+    <t>J927</t>
   </si>
   <si>
     <t>J930</t>
   </si>
   <si>
+    <t>J935</t>
+  </si>
+  <si>
     <t>J937</t>
   </si>
   <si>
+    <t>J945</t>
+  </si>
+  <si>
     <t>J953</t>
   </si>
   <si>
     <t>J956</t>
   </si>
   <si>
-    <t>J965</t>
-  </si>
-  <si>
     <t>J971</t>
   </si>
   <si>
-    <t>J981</t>
-  </si>
-  <si>
-    <t>R955</t>
-  </si>
-  <si>
-    <t>S617</t>
-  </si>
-  <si>
-    <t>S643</t>
-  </si>
-  <si>
-    <t>S656</t>
-  </si>
-  <si>
-    <t>S661</t>
-  </si>
-  <si>
-    <t>S728</t>
+    <t>J972</t>
+  </si>
+  <si>
+    <t>R521</t>
+  </si>
+  <si>
+    <t>S615</t>
+  </si>
+  <si>
+    <t>S637</t>
   </si>
   <si>
     <t>S707</t>
   </si>
   <si>
-    <t>S731</t>
-  </si>
-  <si>
-    <t>S737</t>
-  </si>
-  <si>
-    <t>S801#2</t>
-  </si>
-  <si>
-    <t>S807</t>
-  </si>
-  <si>
-    <t>S836#1</t>
-  </si>
-  <si>
     <t>S837#1</t>
   </si>
   <si>
     <t>S838#M</t>
-  </si>
-  <si>
-    <t>S841</t>
-  </si>
-  <si>
-    <t>S874#16K</t>
-  </si>
-  <si>
-    <t>S985</t>
   </si>
 </sst>
 </file>
@@ -631,7 +547,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -685,61 +601,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -747,7 +608,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -769,362 +630,272 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v3.0.0 : work from A to Z --> TODO : next steps is to then Read the Assembly list option
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damien\Documents\GitHub\DataSheetExtractor_v1.1.0\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB8BD6F-C6A3-475C-A3B0-630EBBA4698A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>Référence</t>
   </si>
@@ -47,21 +41,21 @@
     <t>H060</t>
   </si>
   <si>
+    <t>H115</t>
+  </si>
+  <si>
     <t>H089</t>
   </si>
   <si>
-    <t>H115</t>
-  </si>
-  <si>
     <t>J146</t>
   </si>
   <si>
+    <t>J193</t>
+  </si>
+  <si>
     <t>J311</t>
   </si>
   <si>
-    <t>J193</t>
-  </si>
-  <si>
     <t>H190</t>
   </si>
   <si>
@@ -110,7 +104,7 @@
     <t>H590#90E0</t>
   </si>
   <si>
-    <t>J535#655B</t>
+    <t>0303~J535#655B</t>
   </si>
   <si>
     <t>J541#60V8</t>
@@ -125,7 +119,7 @@
     <t>J572#656F</t>
   </si>
   <si>
-    <t>J599#6569</t>
+    <t>J5994#6569</t>
   </si>
   <si>
     <t>H501#G103</t>
@@ -137,12 +131,12 @@
     <t>H990#32K</t>
   </si>
   <si>
+    <t>J674</t>
+  </si>
+  <si>
     <t>J721</t>
   </si>
   <si>
-    <t>J674</t>
-  </si>
-  <si>
     <t>J728</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>J819</t>
   </si>
   <si>
-    <t>J828</t>
-  </si>
-  <si>
     <t>J829</t>
   </si>
   <si>
@@ -194,18 +185,9 @@
     <t>J836</t>
   </si>
   <si>
-    <t>J838</t>
-  </si>
-  <si>
-    <t>J841</t>
-  </si>
-  <si>
     <t>J842</t>
   </si>
   <si>
-    <t>J846</t>
-  </si>
-  <si>
     <t>J848</t>
   </si>
   <si>
@@ -224,12 +206,6 @@
     <t>J876</t>
   </si>
   <si>
-    <t>J882</t>
-  </si>
-  <si>
-    <t>J887</t>
-  </si>
-  <si>
     <t>J890</t>
   </si>
   <si>
@@ -242,6 +218,9 @@
     <t>J895</t>
   </si>
   <si>
+    <t>J913</t>
+  </si>
+  <si>
     <t>J917</t>
   </si>
   <si>
@@ -275,6 +254,9 @@
     <t>S617</t>
   </si>
   <si>
+    <t>S643</t>
+  </si>
+  <si>
     <t>S656</t>
   </si>
   <si>
@@ -290,32 +272,17 @@
     <t>S731</t>
   </si>
   <si>
-    <t>S737</t>
-  </si>
-  <si>
     <t>S837#1</t>
   </si>
   <si>
-    <t>S841</t>
-  </si>
-  <si>
-    <t>S874#16K</t>
-  </si>
-  <si>
     <t>S985</t>
-  </si>
-  <si>
-    <t>J913</t>
-  </si>
-  <si>
-    <t>S643</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,28 +311,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -407,7 +365,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,27 +397,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -491,24 +431,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -684,20 +606,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -705,102 +621,102 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -811,22 +727,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -840,365 +748,319 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>